<commit_message>
New BCI data files
</commit_message>
<xml_diff>
--- a/TTestApp/ms_to_hr.xlsx
+++ b/TTestApp/ms_to_hr.xlsx
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -396,63 +396,76 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <f>1/C1</f>
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>5719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <f>F1-F2</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f>F3</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
         <f>C4*C2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1">
         <f>1/C5</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3227513227513228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1">
         <f>C7*60</f>
-        <v>30</v>
+        <v>79.365079365079367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change pumping, delay after
</commit_message>
<xml_diff>
--- a/TTestApp/ms_to_hr.xlsx
+++ b/TTestApp/ms_to_hr.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -501,43 +501,31 @@
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>2931</v>
-      </c>
-      <c r="B17" s="1">
-        <v>142</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" ref="C17:C19" si="0">A17/B17</f>
-        <v>20.640845070422536</v>
-      </c>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>2941</v>
+        <v>4286</v>
       </c>
       <c r="B18" s="1">
-        <v>142</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>20.711267605633804</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>3010</v>
+        <v>3960</v>
       </c>
       <c r="B19" s="1">
-        <v>146</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>20.616438356164384</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="3">
+        <v>4000</v>
+      </c>
+      <c r="B20" s="1">
+        <v>195</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -545,25 +533,25 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f>SUM(A15:A21)</f>
-        <v>8882</v>
+        <v>12246</v>
       </c>
       <c r="B22" s="1">
         <f>SUM(B15:B21)</f>
-        <v>430</v>
+        <v>593</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f>A22/3</f>
-        <v>2960.6666666666665</v>
+        <v>4082</v>
       </c>
       <c r="B23" s="1">
         <f>B22/3</f>
-        <v>143.33333333333334</v>
+        <v>197.66666666666666</v>
       </c>
       <c r="C23" s="1">
         <f>A23/B23</f>
-        <v>20.655813953488369</v>
+        <v>20.650927487352448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unused from WaveDetector
</commit_message>
<xml_diff>
--- a/TTestApp/ms_to_hr.xlsx
+++ b/TTestApp/ms_to_hr.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
-        <v>162</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
       </c>
       <c r="C5" s="1">
         <f>C4*C2</f>
-        <v>0.64800000000000002</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
       </c>
       <c r="C7" s="1">
         <f>1/C5</f>
-        <v>1.5432098765432098</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -471,19 +471,19 @@
       </c>
       <c r="C8" s="1">
         <f>C7*60</f>
-        <v>92.592592592592595</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
         <f>C8/60</f>
-        <v>1.5432098765432098</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="1">
         <f>1/E8</f>
-        <v>0.64800000000000002</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <f>F8*C1</f>
-        <v>162</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove Spline and Filters
</commit_message>
<xml_diff>
--- a/TTestApp/ms_to_hr.xlsx
+++ b/TTestApp/ms_to_hr.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
-        <v>500</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
       </c>
       <c r="C5" s="1">
         <f>C4*C2</f>
-        <v>2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
       </c>
       <c r="C7" s="1">
         <f>1/C5</f>
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -471,19 +471,19 @@
       </c>
       <c r="C8" s="1">
         <f>C7*60</f>
-        <v>30</v>
+        <v>750</v>
       </c>
       <c r="E8" s="1">
         <f>C8/60</f>
-        <v>0.5</v>
+        <v>12.5</v>
       </c>
       <c r="F8" s="1">
         <f>1/E8</f>
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="G8" s="1">
         <f>F8*C1</f>
-        <v>500</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
5 bytes in packet. 2 curves.
</commit_message>
<xml_diff>
--- a/TTestApp/ms_to_hr.xlsx
+++ b/TTestApp/ms_to_hr.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Частота дискретизации</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>mmHg</t>
+  </si>
+  <si>
+    <t>уд/мин</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -403,12 +406,12 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -417,13 +420,13 @@
         <v>5908</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <f>1/C1</f>
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -432,22 +435,25 @@
         <v>5719</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" s="1">
         <f>F1-F2</f>
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -455,8 +461,22 @@
         <f>C4*C2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>60</v>
+      </c>
+      <c r="K5" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>400</v>
+      </c>
+      <c r="K6" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -465,7 +485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -483,10 +503,10 @@
       </c>
       <c r="G8" s="1">
         <f>F8*C1</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -494,10 +514,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>